<commit_message>
fixed a bug of Bard
</commit_message>
<xml_diff>
--- a/Output/TriggerLines/时间轴 p4s门神 诗人 被窝两分半第二轮团辅.xlsx
+++ b/Output/TriggerLines/时间轴 p4s门神 诗人 被窝两分半第二轮团辅.xlsx
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="68">
   <si>
     <t>作者:</t>
   </si>
@@ -332,12 +332,6 @@
   </si>
   <si>
     <t>Action:SwitchBurst:是否允许爆发</t>
-  </si>
-  <si>
-    <t>#第二轮先切歌,再延后团辅</t>
-  </si>
-  <si>
-    <t>Action:CastAbility:优先使用指定能力技</t>
   </si>
   <si>
     <t>#回场中开爆发,对齐150秒的团辅</t>
@@ -357,10 +351,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -379,35 +373,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -421,13 +408,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -438,7 +418,38 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -452,24 +463,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -485,38 +488,29 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -584,175 +578,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -763,24 +757,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -795,6 +771,65 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -817,49 +852,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -871,10 +865,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -883,133 +877,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1443,10 +1437,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AQ43"/>
+  <dimension ref="A1:AQ40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1721,16 +1715,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:6">
-      <c r="B13" s="1" t="s">
+    <row r="13" spans="2:5">
+      <c r="B13" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="16"/>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="3:6">
       <c r="C14" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>57</v>
@@ -1739,97 +1732,72 @@
         <v>58</v>
       </c>
       <c r="F14" s="1">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="3:6">
       <c r="C15" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>59</v>
       </c>
       <c r="E15" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="15">
-        <v>3559</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="B16" s="14" t="s">
-        <v>66</v>
-      </c>
       <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="3:6">
+      <c r="F16" s="17"/>
+    </row>
+    <row r="17" spans="3:8">
       <c r="C17" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="1">
-        <v>145</v>
+        <v>66</v>
+      </c>
+      <c r="F17" s="17">
+        <v>10742</v>
+      </c>
+      <c r="G17" s="1">
+        <v>50.5</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="3:6">
       <c r="C18" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E18" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" s="16">
+      <c r="E18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
-      <c r="B19" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" s="1"/>
+    <row r="19" spans="6:6">
       <c r="F19" s="17"/>
     </row>
-    <row r="20" spans="3:8">
-      <c r="C20" s="1">
-        <v>5</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F20" s="17">
-        <v>10742</v>
-      </c>
-      <c r="G20" s="1">
-        <v>50.5</v>
-      </c>
-      <c r="H20" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6">
-      <c r="C21" s="1">
-        <v>5</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F21" s="17">
-        <v>1</v>
-      </c>
+    <row r="20" spans="6:6">
+      <c r="F20" s="17"/>
+    </row>
+    <row r="21" spans="6:6">
+      <c r="F21" s="17"/>
     </row>
     <row r="22" spans="6:6">
       <c r="F22" s="17"/>
@@ -1887,28 +1855,19 @@
     </row>
     <row r="40" spans="6:6">
       <c r="F40" s="17"/>
-    </row>
-    <row r="41" spans="6:6">
-      <c r="F41" s="17"/>
-    </row>
-    <row r="42" spans="6:6">
-      <c r="F42" s="17"/>
-    </row>
-    <row r="43" spans="6:6">
-      <c r="F43" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A5:B5"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D13 D14 D15 D11:D12 D17:D18 D19:D21">
-      <formula1>"Cond,Action"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
       <formula1>$C$4:$AQ$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13 E14 E15 E11:E12 E17:E18 E19:E21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:D12 D14:D15 D16:D18">
+      <formula1>"Cond,Action"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11:E12 E14:E15 E16:E18">
       <formula1>'[1]#参数说明'!#REF!</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>